<commit_message>
update data and filter in R code; change css in html; remove pubmed link in js
</commit_message>
<xml_diff>
--- a/data/adc_2019_v4.xlsx
+++ b/data/adc_2019_v4.xlsx
@@ -485,7 +485,7 @@
     <t>glioma</t>
   </si>
   <si>
-    <t>skin</t>
+    <t>merkel</t>
   </si>
   <si>
     <t>neuroblastoma</t>
@@ -500,42 +500,45 @@
     <t>hemato</t>
   </si>
   <si>
-    <t>target-tumor interaction</t>
-  </si>
-  <si>
-    <t>target discovery</t>
+    <t>target-tumor</t>
+  </si>
+  <si>
+    <t>discovery</t>
   </si>
   <si>
     <t>payload</t>
   </si>
   <si>
+    <t>synergy</t>
+  </si>
+  <si>
+    <t>resistance</t>
+  </si>
+  <si>
+    <t>payload-linker</t>
+  </si>
+  <si>
+    <t>linker</t>
+  </si>
+  <si>
+    <t>platform</t>
+  </si>
+  <si>
+    <t>phase 1</t>
+  </si>
+  <si>
+    <t>academia</t>
+  </si>
+  <si>
+    <t>pharma</t>
+  </si>
+  <si>
+    <t>single</t>
+  </si>
+  <si>
     <t>combo</t>
   </si>
   <si>
-    <t>resistance to ADC</t>
-  </si>
-  <si>
-    <t>payload-linker</t>
-  </si>
-  <si>
-    <t>linker</t>
-  </si>
-  <si>
-    <t>platform</t>
-  </si>
-  <si>
-    <t>phase 1</t>
-  </si>
-  <si>
-    <t>academia</t>
-  </si>
-  <si>
-    <t>pharma</t>
-  </si>
-  <si>
-    <t>single</t>
-  </si>
-  <si>
     <t>clinical</t>
   </si>
   <si>
@@ -2019,9 +2022,6 @@
   </si>
   <si>
     <t>Photoimmunotherapy</t>
-  </si>
-  <si>
-    <t>resistance</t>
   </si>
   <si>
     <t>Chemotherapy</t>
@@ -2655,37 +2655,37 @@
         <v>173</v>
       </c>
       <c r="H2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="I2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="J2" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="K2" t="e">
         <v>#N/A</v>
       </c>
       <c r="L2" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="M2" t="e">
         <v>#N/A</v>
       </c>
       <c r="N2" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="O2" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="P2" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="Q2" t="s">
         <v>104</v>
       </c>
       <c r="R2" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="S2" t="s">
         <v>707</v>
@@ -2720,37 +2720,37 @@
         <v>173</v>
       </c>
       <c r="H3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="I3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="J3" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="K3" t="e">
         <v>#N/A</v>
       </c>
       <c r="L3" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="M3" t="e">
         <v>#N/A</v>
       </c>
       <c r="N3" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="O3" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="P3" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="Q3" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="R3" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="S3" t="e">
         <v>#N/A</v>
@@ -2785,34 +2785,34 @@
         <v>173</v>
       </c>
       <c r="H4" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I4" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="J4" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="K4" t="e">
         <v>#N/A</v>
       </c>
       <c r="L4" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="M4" t="e">
         <v>#N/A</v>
       </c>
       <c r="N4" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="O4" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="P4" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="Q4" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="R4" t="e">
         <v>#N/A</v>
@@ -2850,43 +2850,43 @@
         <v>173</v>
       </c>
       <c r="H5" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="J5" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="K5" t="e">
         <v>#N/A</v>
       </c>
       <c r="L5" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="M5" t="e">
         <v>#N/A</v>
       </c>
       <c r="N5" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="O5" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="P5" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="Q5" t="s">
         <v>107</v>
       </c>
       <c r="R5" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="S5" t="e">
         <v>#N/A</v>
       </c>
       <c r="T5" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="U5" t="s">
         <v>755</v>
@@ -2915,34 +2915,34 @@
         <v>173</v>
       </c>
       <c r="H6" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I6" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="J6" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="K6" t="e">
         <v>#N/A</v>
       </c>
       <c r="L6" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="M6" t="e">
         <v>#N/A</v>
       </c>
       <c r="N6" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="O6" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="P6" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="Q6" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="R6" t="s">
         <v>108</v>
@@ -2951,7 +2951,7 @@
         <v>708</v>
       </c>
       <c r="T6" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="U6" t="s">
         <v>756</v>
@@ -2980,43 +2980,43 @@
         <v>173</v>
       </c>
       <c r="H7" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I7" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="J7" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="K7" t="e">
         <v>#N/A</v>
       </c>
       <c r="L7" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="M7" t="e">
         <v>#N/A</v>
       </c>
       <c r="N7" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="O7" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="P7" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="Q7" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="R7" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="S7" t="s">
         <v>709</v>
       </c>
       <c r="T7" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="U7" t="s">
         <v>757</v>
@@ -3045,37 +3045,37 @@
         <v>173</v>
       </c>
       <c r="H8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="J8" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="K8" t="e">
         <v>#N/A</v>
       </c>
       <c r="L8" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="M8" t="e">
         <v>#N/A</v>
       </c>
       <c r="N8" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="O8" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="P8" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="Q8" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="R8" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="S8" t="s">
         <v>710</v>
@@ -3110,37 +3110,37 @@
         <v>173</v>
       </c>
       <c r="H9" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I9" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="J9" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="K9" t="e">
         <v>#N/A</v>
       </c>
       <c r="L9" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="M9" t="e">
         <v>#N/A</v>
       </c>
       <c r="N9" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="O9" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="P9" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="Q9" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="R9" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="S9" t="e">
         <v>#N/A</v>
@@ -3175,31 +3175,31 @@
         <v>173</v>
       </c>
       <c r="H10" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I10" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J10" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="K10" t="e">
         <v>#N/A</v>
       </c>
       <c r="L10" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="M10" t="e">
         <v>#N/A</v>
       </c>
       <c r="N10" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="O10" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="P10" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="Q10" t="s">
         <v>112</v>
@@ -3240,34 +3240,34 @@
         <v>173</v>
       </c>
       <c r="H11" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I11" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="J11" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="K11" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="L11" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="M11" t="e">
         <v>#N/A</v>
       </c>
       <c r="N11" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="O11" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="P11" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="Q11" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="R11" t="e">
         <v>#N/A</v>
@@ -3276,7 +3276,7 @@
         <v>#N/A</v>
       </c>
       <c r="T11" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="U11" t="s">
         <v>761</v>
@@ -3302,46 +3302,46 @@
         <v>172</v>
       </c>
       <c r="G12" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="H12" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I12" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="J12" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="K12" t="e">
         <v>#N/A</v>
       </c>
       <c r="L12" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="M12" t="e">
         <v>#N/A</v>
       </c>
       <c r="N12" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="O12" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="P12" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="Q12" t="s">
         <v>114</v>
       </c>
       <c r="R12" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="S12" t="s">
         <v>711</v>
       </c>
       <c r="T12" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="U12" t="s">
         <v>762</v>
@@ -3370,37 +3370,37 @@
         <v>173</v>
       </c>
       <c r="H13" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="I13" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="J13" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="K13" t="e">
         <v>#N/A</v>
       </c>
       <c r="L13" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="M13" t="e">
         <v>#N/A</v>
       </c>
       <c r="N13" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="O13" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="P13" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="Q13" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="R13" t="s">
-        <v>669</v>
+        <v>166</v>
       </c>
       <c r="S13" t="e">
         <v>#N/A</v>
@@ -3435,34 +3435,34 @@
         <v>173</v>
       </c>
       <c r="H14" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="I14" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="J14" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="K14" t="e">
         <v>#N/A</v>
       </c>
       <c r="L14" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="M14" t="e">
         <v>#N/A</v>
       </c>
       <c r="N14" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="O14" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="P14" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="Q14" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="R14" t="s">
         <v>670</v>
@@ -3471,7 +3471,7 @@
         <v>712</v>
       </c>
       <c r="T14" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="U14" t="s">
         <v>764</v>
@@ -3500,40 +3500,40 @@
         <v>173</v>
       </c>
       <c r="H15" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="I15" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="J15" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="K15" t="e">
         <v>#N/A</v>
       </c>
       <c r="L15" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="M15" t="e">
         <v>#N/A</v>
       </c>
       <c r="N15" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="O15" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="P15" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="Q15" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="R15" t="s">
         <v>671</v>
       </c>
       <c r="S15" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="T15" t="e">
         <v>#N/A</v>
@@ -3565,31 +3565,31 @@
         <v>173</v>
       </c>
       <c r="H16" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I16" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="J16" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="K16" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="L16" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="M16" t="e">
         <v>#N/A</v>
       </c>
       <c r="N16" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="O16" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="P16" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="Q16" t="s">
         <v>114</v>
@@ -3598,10 +3598,10 @@
         <v>672</v>
       </c>
       <c r="S16" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="T16" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="U16" t="s">
         <v>766</v>
@@ -3630,34 +3630,34 @@
         <v>173</v>
       </c>
       <c r="H17" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I17" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="J17" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="K17" t="e">
         <v>#N/A</v>
       </c>
       <c r="L17" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="M17" t="e">
         <v>#N/A</v>
       </c>
       <c r="N17" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="O17" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="P17" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="Q17" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="R17" t="s">
         <v>673</v>
@@ -3695,40 +3695,40 @@
         <v>173</v>
       </c>
       <c r="H18" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I18" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="J18" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="K18" t="e">
         <v>#N/A</v>
       </c>
       <c r="L18" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="M18" t="e">
         <v>#N/A</v>
       </c>
       <c r="N18" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="O18" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="P18" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="Q18" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="R18" t="s">
         <v>674</v>
       </c>
       <c r="S18" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="T18" t="e">
         <v>#N/A</v>
@@ -3760,37 +3760,37 @@
         <v>173</v>
       </c>
       <c r="H19" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I19" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="J19" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="K19" t="e">
         <v>#N/A</v>
       </c>
       <c r="L19" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="M19" t="e">
         <v>#N/A</v>
       </c>
       <c r="N19" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="O19" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="P19" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="Q19" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="R19" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="S19" t="e">
         <v>#N/A</v>
@@ -3825,34 +3825,34 @@
         <v>173</v>
       </c>
       <c r="H20" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="I20" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="J20" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="K20" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="L20" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="M20" t="e">
         <v>#N/A</v>
       </c>
       <c r="N20" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="O20" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="P20" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="Q20" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="R20" t="s">
         <v>675</v>
@@ -3890,37 +3890,37 @@
         <v>173</v>
       </c>
       <c r="H21" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="I21" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="J21" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="K21" t="e">
         <v>#N/A</v>
       </c>
       <c r="L21" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="M21" t="e">
         <v>#N/A</v>
       </c>
       <c r="N21" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="O21" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="P21" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="Q21" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="R21" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="S21" t="s">
         <v>713</v>
@@ -3955,40 +3955,40 @@
         <v>173</v>
       </c>
       <c r="H22" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="I22" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="J22" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="K22" t="e">
         <v>#N/A</v>
       </c>
       <c r="L22" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="M22" t="e">
         <v>#N/A</v>
       </c>
       <c r="N22" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="O22" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="P22" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="Q22" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="R22" t="s">
         <v>676</v>
       </c>
       <c r="S22" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="T22" t="e">
         <v>#N/A</v>
@@ -4020,40 +4020,40 @@
         <v>173</v>
       </c>
       <c r="H23" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I23" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="J23" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="K23" t="e">
         <v>#N/A</v>
       </c>
       <c r="L23" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="M23" t="e">
         <v>#N/A</v>
       </c>
       <c r="N23" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="O23" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="P23" t="s">
         <v>119</v>
       </c>
       <c r="Q23" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="R23" t="s">
         <v>677</v>
       </c>
       <c r="S23" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="T23" t="s">
         <v>742</v>
@@ -4085,40 +4085,40 @@
         <v>173</v>
       </c>
       <c r="H24" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I24" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="J24" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="K24" t="e">
         <v>#N/A</v>
       </c>
       <c r="L24" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="M24" t="e">
         <v>#N/A</v>
       </c>
       <c r="N24" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="O24" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="P24" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="Q24" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="R24" t="s">
         <v>678</v>
       </c>
       <c r="S24" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="T24" t="s">
         <v>743</v>
@@ -4150,40 +4150,40 @@
         <v>173</v>
       </c>
       <c r="H25" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I25" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="J25" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="K25" t="e">
         <v>#N/A</v>
       </c>
       <c r="L25" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="M25" t="e">
         <v>#N/A</v>
       </c>
       <c r="N25" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="O25" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="P25" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="Q25" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="R25" t="s">
         <v>679</v>
       </c>
       <c r="S25" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="T25" t="e">
         <v>#N/A</v>
@@ -4212,40 +4212,40 @@
         <v>172</v>
       </c>
       <c r="G26" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="H26" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I26" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="J26" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="K26" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="L26" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="M26" t="e">
         <v>#N/A</v>
       </c>
       <c r="N26" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="O26" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="P26" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="Q26" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="R26" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="S26" t="s">
         <v>714</v>
@@ -4280,31 +4280,31 @@
         <v>173</v>
       </c>
       <c r="H27" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I27" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="J27" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="K27" t="e">
         <v>#N/A</v>
       </c>
       <c r="L27" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="M27" t="e">
         <v>#N/A</v>
       </c>
       <c r="N27" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="O27" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="P27" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="Q27" t="s">
         <v>107</v>
@@ -4316,7 +4316,7 @@
         <v>715</v>
       </c>
       <c r="T27" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="U27" t="s">
         <v>777</v>
@@ -4345,37 +4345,37 @@
         <v>173</v>
       </c>
       <c r="H28" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I28" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="J28" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="K28" t="e">
         <v>#N/A</v>
       </c>
       <c r="L28" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="M28" t="e">
         <v>#N/A</v>
       </c>
       <c r="N28" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="O28" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="P28" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="Q28" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="R28" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="S28" t="s">
         <v>716</v>
@@ -4410,37 +4410,37 @@
         <v>173</v>
       </c>
       <c r="H29" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I29" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="J29" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="K29" t="e">
         <v>#N/A</v>
       </c>
       <c r="L29" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="M29" t="e">
         <v>#N/A</v>
       </c>
       <c r="N29" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="O29" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="P29" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="Q29" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="R29" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="S29" t="s">
         <v>717</v>
@@ -4475,34 +4475,34 @@
         <v>173</v>
       </c>
       <c r="H30" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="I30" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="J30" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="K30" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="L30" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="M30" t="e">
         <v>#N/A</v>
       </c>
       <c r="N30" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="O30" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="P30" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="Q30" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="R30" t="s">
         <v>681</v>
@@ -4540,37 +4540,37 @@
         <v>173</v>
       </c>
       <c r="H31" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I31" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="J31" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="K31" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="L31" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="M31" t="e">
         <v>#N/A</v>
       </c>
       <c r="N31" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="O31" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="P31" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="Q31" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="R31" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="S31" t="s">
         <v>719</v>
@@ -4605,34 +4605,34 @@
         <v>173</v>
       </c>
       <c r="H32" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I32" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="J32" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="K32" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="L32" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="M32" t="e">
         <v>#N/A</v>
       </c>
       <c r="N32" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="O32" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="P32" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="Q32" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R32" t="e">
         <v>#N/A</v>
@@ -4641,7 +4641,7 @@
         <v>#N/A</v>
       </c>
       <c r="T32" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="U32" t="s">
         <v>782</v>
@@ -4670,40 +4670,40 @@
         <v>173</v>
       </c>
       <c r="H33" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I33" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J33" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="K33" t="e">
         <v>#N/A</v>
       </c>
       <c r="L33" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="M33" t="e">
         <v>#N/A</v>
       </c>
       <c r="N33" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="O33" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="P33" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="Q33" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="R33" t="s">
         <v>682</v>
       </c>
       <c r="S33" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="T33" t="s">
         <v>745</v>
@@ -4735,43 +4735,43 @@
         <v>173</v>
       </c>
       <c r="H34" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="I34" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="J34" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="K34" t="e">
         <v>#N/A</v>
       </c>
       <c r="L34" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="M34" t="e">
         <v>#N/A</v>
       </c>
       <c r="N34" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="O34" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="P34" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="Q34" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="R34" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="S34" t="e">
         <v>#N/A</v>
       </c>
       <c r="T34" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="U34" t="s">
         <v>784</v>
@@ -4800,34 +4800,34 @@
         <v>173</v>
       </c>
       <c r="H35" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I35" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="J35" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="K35" t="e">
         <v>#N/A</v>
       </c>
       <c r="L35" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="M35" t="e">
         <v>#N/A</v>
       </c>
       <c r="N35" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="O35" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="P35" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="Q35" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="R35" t="s">
         <v>126</v>
@@ -4865,31 +4865,31 @@
         <v>173</v>
       </c>
       <c r="H36" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I36" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="J36" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="K36" t="e">
         <v>#N/A</v>
       </c>
       <c r="L36" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="M36" t="e">
         <v>#N/A</v>
       </c>
       <c r="N36" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="O36" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="P36" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="Q36" t="s">
         <v>107</v>
@@ -4898,10 +4898,10 @@
         <v>683</v>
       </c>
       <c r="S36" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="T36" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="U36" t="s">
         <v>786</v>
@@ -4930,34 +4930,34 @@
         <v>173</v>
       </c>
       <c r="H37" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="I37" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="J37" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="K37" t="e">
         <v>#N/A</v>
       </c>
       <c r="L37" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="M37" t="e">
         <v>#N/A</v>
       </c>
       <c r="N37" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="O37" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="P37" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="Q37" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="R37" t="s">
         <v>684</v>
@@ -4992,43 +4992,43 @@
         <v>171</v>
       </c>
       <c r="G38" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="H38" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I38" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="J38" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="K38" t="e">
         <v>#N/A</v>
       </c>
       <c r="L38" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="M38" t="e">
         <v>#N/A</v>
       </c>
       <c r="N38" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="O38" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="P38" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="Q38" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="R38" t="s">
         <v>685</v>
       </c>
       <c r="S38" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="T38" t="s">
         <v>747</v>
@@ -5060,34 +5060,34 @@
         <v>173</v>
       </c>
       <c r="H39" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I39" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="J39" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="K39" t="e">
         <v>#N/A</v>
       </c>
       <c r="L39" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="M39" t="e">
         <v>#N/A</v>
       </c>
       <c r="N39" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="O39" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="P39" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="Q39" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="R39" t="s">
         <v>686</v>
@@ -5125,34 +5125,34 @@
         <v>173</v>
       </c>
       <c r="H40" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I40" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="J40" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="K40" t="e">
         <v>#N/A</v>
       </c>
       <c r="L40" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="M40" t="e">
         <v>#N/A</v>
       </c>
       <c r="N40" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="O40" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="P40" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="Q40" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="R40" t="s">
         <v>107</v>
@@ -5161,7 +5161,7 @@
         <v>721</v>
       </c>
       <c r="T40" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="U40" t="s">
         <v>790</v>
@@ -5190,37 +5190,37 @@
         <v>173</v>
       </c>
       <c r="H41" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="I41" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="J41" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="K41" t="e">
         <v>#N/A</v>
       </c>
       <c r="L41" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="M41" t="e">
         <v>#N/A</v>
       </c>
       <c r="N41" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="O41" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="P41" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="Q41" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="R41" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="S41" t="s">
         <v>722</v>
@@ -5252,37 +5252,37 @@
         <v>171</v>
       </c>
       <c r="G42" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="H42" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="I42" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="J42" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="K42" t="e">
         <v>#N/A</v>
       </c>
       <c r="L42" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="M42" t="e">
         <v>#N/A</v>
       </c>
       <c r="N42" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="O42" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="P42" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="Q42" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="R42" t="s">
         <v>107</v>
@@ -5291,7 +5291,7 @@
         <v>698</v>
       </c>
       <c r="T42" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="U42" t="s">
         <v>792</v>
@@ -5320,37 +5320,37 @@
         <v>173</v>
       </c>
       <c r="H43" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="I43" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="J43" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="K43" t="e">
         <v>#N/A</v>
       </c>
       <c r="L43" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="M43" t="e">
         <v>#N/A</v>
       </c>
       <c r="N43" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="O43" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="P43" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="Q43" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="R43" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="S43" t="s">
         <v>723</v>
@@ -5385,31 +5385,31 @@
         <v>173</v>
       </c>
       <c r="H44" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I44" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="J44" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="K44" t="e">
         <v>#N/A</v>
       </c>
       <c r="L44" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="M44" t="e">
         <v>#N/A</v>
       </c>
       <c r="N44" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="O44" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="P44" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="Q44" t="s">
         <v>118</v>
@@ -5450,43 +5450,43 @@
         <v>173</v>
       </c>
       <c r="H45" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I45" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="J45" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="K45" t="e">
         <v>#N/A</v>
       </c>
       <c r="L45" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="M45" t="e">
         <v>#N/A</v>
       </c>
       <c r="N45" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="O45" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="P45" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="Q45" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="R45" t="s">
         <v>688</v>
       </c>
       <c r="S45" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="T45" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="U45" t="s">
         <v>795</v>
@@ -5512,34 +5512,34 @@
         <v>171</v>
       </c>
       <c r="G46" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="H46" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I46" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="J46" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="K46" t="e">
         <v>#N/A</v>
       </c>
       <c r="L46" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="M46" t="e">
         <v>#N/A</v>
       </c>
       <c r="N46" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="O46" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="P46" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="Q46" t="s">
         <v>107</v>
@@ -5551,7 +5551,7 @@
         <v>724</v>
       </c>
       <c r="T46" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="U46" t="s">
         <v>796</v>
@@ -5580,34 +5580,34 @@
         <v>173</v>
       </c>
       <c r="H47" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I47" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="J47" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="K47" t="e">
         <v>#N/A</v>
       </c>
       <c r="L47" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="M47" t="e">
         <v>#N/A</v>
       </c>
       <c r="N47" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="O47" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="P47" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="Q47" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="R47" t="e">
         <v>#N/A</v>
@@ -5642,37 +5642,37 @@
         <v>171</v>
       </c>
       <c r="G48" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="H48" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="I48" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="J48" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="K48" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="L48" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="M48" t="e">
         <v>#N/A</v>
       </c>
       <c r="N48" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="O48" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="P48" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="Q48" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="R48" t="s">
         <v>690</v>
@@ -5681,7 +5681,7 @@
         <v>725</v>
       </c>
       <c r="T48" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="U48" t="s">
         <v>798</v>
@@ -5710,40 +5710,40 @@
         <v>173</v>
       </c>
       <c r="H49" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="I49" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="J49" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="K49" t="e">
         <v>#N/A</v>
       </c>
       <c r="L49" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="M49" t="e">
         <v>#N/A</v>
       </c>
       <c r="N49" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="O49" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="P49" t="s">
+        <v>592</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>590</v>
+      </c>
+      <c r="R49" t="s">
         <v>591</v>
       </c>
-      <c r="Q49" t="s">
-        <v>589</v>
-      </c>
-      <c r="R49" t="s">
-        <v>590</v>
-      </c>
       <c r="S49" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="T49" t="e">
         <v>#N/A</v>
@@ -5775,37 +5775,37 @@
         <v>173</v>
       </c>
       <c r="H50" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I50" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="J50" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="K50" t="e">
         <v>#N/A</v>
       </c>
       <c r="L50" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="M50" t="e">
         <v>#N/A</v>
       </c>
       <c r="N50" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="O50" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="P50" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="Q50" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="R50" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="S50" t="s">
         <v>726</v>
@@ -5840,40 +5840,40 @@
         <v>173</v>
       </c>
       <c r="H51" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I51" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="J51" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="K51" t="e">
         <v>#N/A</v>
       </c>
       <c r="L51" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="M51" t="e">
         <v>#N/A</v>
       </c>
       <c r="N51" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="O51" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="P51" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="Q51" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="R51" t="s">
         <v>691</v>
       </c>
       <c r="S51" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="T51" t="e">
         <v>#N/A</v>
@@ -5905,37 +5905,37 @@
         <v>173</v>
       </c>
       <c r="H52" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="I52" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="J52" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="K52" t="e">
         <v>#N/A</v>
       </c>
       <c r="L52" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="M52" t="e">
         <v>#N/A</v>
       </c>
       <c r="N52" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="O52" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="P52" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="Q52" t="s">
         <v>133</v>
       </c>
       <c r="R52" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="S52" t="s">
         <v>727</v>
@@ -5970,43 +5970,43 @@
         <v>173</v>
       </c>
       <c r="H53" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I53" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J53" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="K53" t="e">
         <v>#N/A</v>
       </c>
       <c r="L53" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="M53" t="e">
         <v>#N/A</v>
       </c>
       <c r="N53" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="O53" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="P53" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="Q53" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="R53" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="S53" t="s">
         <v>728</v>
       </c>
       <c r="T53" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="U53" t="s">
         <v>803</v>
@@ -6035,34 +6035,34 @@
         <v>173</v>
       </c>
       <c r="H54" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I54" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="J54" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="K54" t="e">
         <v>#N/A</v>
       </c>
       <c r="L54" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="M54" t="e">
         <v>#N/A</v>
       </c>
       <c r="N54" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="O54" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="P54" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="Q54" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="R54" t="s">
         <v>691</v>
@@ -6097,43 +6097,43 @@
         <v>172</v>
       </c>
       <c r="G55" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="H55" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I55" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="J55" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="K55" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="L55" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="M55" t="e">
         <v>#N/A</v>
       </c>
       <c r="N55" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="O55" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="P55" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="Q55" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="R55" t="s">
         <v>692</v>
       </c>
       <c r="S55" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="T55" t="s">
         <v>738</v>
@@ -6165,31 +6165,31 @@
         <v>173</v>
       </c>
       <c r="H56" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="I56" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="J56" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="K56" t="e">
         <v>#N/A</v>
       </c>
       <c r="L56" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="M56" t="e">
         <v>#N/A</v>
       </c>
       <c r="N56" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="O56" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="P56" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="Q56" t="e">
         <v>#N/A</v>
@@ -6230,40 +6230,40 @@
         <v>173</v>
       </c>
       <c r="H57" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I57" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="J57" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="K57" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="L57" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="M57" t="e">
         <v>#N/A</v>
       </c>
       <c r="N57" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="O57" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="P57" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="Q57" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="R57" t="s">
         <v>693</v>
       </c>
       <c r="S57" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="T57" t="e">
         <v>#N/A</v>
@@ -6295,34 +6295,34 @@
         <v>173</v>
       </c>
       <c r="H58" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="I58" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="J58" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="K58" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="L58" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="M58" t="e">
         <v>#N/A</v>
       </c>
       <c r="N58" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="O58" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="P58" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="Q58" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="R58" t="s">
         <v>694</v>
@@ -6360,40 +6360,40 @@
         <v>173</v>
       </c>
       <c r="H59" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I59" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="J59" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="K59" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="L59" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="M59" t="e">
         <v>#N/A</v>
       </c>
       <c r="N59" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="O59" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="P59" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="Q59" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="R59" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="S59" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="T59" t="s">
         <v>748</v>
@@ -6425,40 +6425,40 @@
         <v>173</v>
       </c>
       <c r="H60" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I60" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="J60" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="K60" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="L60" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="M60" t="e">
         <v>#N/A</v>
       </c>
       <c r="N60" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="O60" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="P60" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="Q60" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="R60" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="S60" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="T60" t="s">
         <v>749</v>
@@ -6490,34 +6490,34 @@
         <v>173</v>
       </c>
       <c r="H61" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="I61" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="J61" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="K61" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="L61" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="M61" t="e">
         <v>#N/A</v>
       </c>
       <c r="N61" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="O61" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="P61" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="Q61" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="R61" t="s">
         <v>695</v>
@@ -6555,34 +6555,34 @@
         <v>173</v>
       </c>
       <c r="H62" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I62" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="J62" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="K62" t="e">
         <v>#N/A</v>
       </c>
       <c r="L62" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="M62" t="e">
         <v>#N/A</v>
       </c>
       <c r="N62" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="O62" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="P62" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="Q62" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="R62" t="s">
         <v>696</v>
@@ -6620,34 +6620,34 @@
         <v>173</v>
       </c>
       <c r="H63" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="I63" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="J63" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="K63" t="e">
         <v>#N/A</v>
       </c>
       <c r="L63" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="M63" t="e">
         <v>#N/A</v>
       </c>
       <c r="N63" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="O63" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="P63" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="Q63" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="R63" t="s">
         <v>697</v>
@@ -6685,37 +6685,37 @@
         <v>173</v>
       </c>
       <c r="H64" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I64" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="J64" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="K64" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="L64" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="M64" t="e">
         <v>#N/A</v>
       </c>
       <c r="N64" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="O64" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="P64" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="Q64" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="R64" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="S64" t="e">
         <v>#N/A</v>
@@ -6750,34 +6750,34 @@
         <v>173</v>
       </c>
       <c r="H65" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I65" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="J65" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="K65" t="e">
         <v>#N/A</v>
       </c>
       <c r="L65" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="M65" t="e">
         <v>#N/A</v>
       </c>
       <c r="N65" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="O65" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="P65" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="Q65" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="R65" t="e">
         <v>#N/A</v>
@@ -6815,34 +6815,34 @@
         <v>173</v>
       </c>
       <c r="H66" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I66" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="J66" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="K66" t="e">
         <v>#N/A</v>
       </c>
       <c r="L66" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="M66" t="e">
         <v>#N/A</v>
       </c>
       <c r="N66" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="O66" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="P66" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="Q66" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="R66" t="s">
         <v>698</v>
@@ -6851,7 +6851,7 @@
         <v>733</v>
       </c>
       <c r="T66" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="U66" t="s">
         <v>816</v>
@@ -6880,40 +6880,40 @@
         <v>173</v>
       </c>
       <c r="H67" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I67" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="J67" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="K67" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="L67" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="M67" t="e">
         <v>#N/A</v>
       </c>
       <c r="N67" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="O67" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="P67" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="Q67" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="R67" t="s">
         <v>699</v>
       </c>
       <c r="S67" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="T67" t="s">
         <v>745</v>
@@ -6942,37 +6942,37 @@
         <v>172</v>
       </c>
       <c r="G68" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="H68" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I68" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="J68" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="K68" t="e">
         <v>#N/A</v>
       </c>
       <c r="L68" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="M68" t="e">
         <v>#N/A</v>
       </c>
       <c r="N68" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="O68" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="P68" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="Q68" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="R68" t="s">
         <v>700</v>
@@ -7010,37 +7010,37 @@
         <v>173</v>
       </c>
       <c r="H69" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I69" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="J69" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="K69" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="L69" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="M69" t="e">
         <v>#N/A</v>
       </c>
       <c r="N69" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="O69" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="P69" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="Q69" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="R69" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="S69" t="s">
         <v>734</v>
@@ -7075,37 +7075,37 @@
         <v>173</v>
       </c>
       <c r="H70" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="I70" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="J70" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="K70" t="e">
         <v>#N/A</v>
       </c>
       <c r="L70" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="M70" t="e">
         <v>#N/A</v>
       </c>
       <c r="N70" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="O70" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="P70" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="Q70" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="R70" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="S70" t="e">
         <v>#N/A</v>
@@ -7140,31 +7140,31 @@
         <v>173</v>
       </c>
       <c r="H71" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I71" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="J71" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="K71" t="e">
         <v>#N/A</v>
       </c>
       <c r="L71" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="M71" t="e">
         <v>#N/A</v>
       </c>
       <c r="N71" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="O71" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="P71" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="Q71" t="s">
         <v>142</v>
@@ -7176,7 +7176,7 @@
         <v>735</v>
       </c>
       <c r="T71" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="U71" t="s">
         <v>821</v>
@@ -7205,31 +7205,31 @@
         <v>173</v>
       </c>
       <c r="H72" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="I72" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="J72" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="K72" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="L72" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="M72" t="e">
         <v>#N/A</v>
       </c>
       <c r="N72" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="O72" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="P72" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="Q72" t="s">
         <v>133</v>
@@ -7270,40 +7270,40 @@
         <v>173</v>
       </c>
       <c r="H73" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I73" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="J73" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="K73" t="e">
         <v>#N/A</v>
       </c>
       <c r="L73" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="M73" t="e">
         <v>#N/A</v>
       </c>
       <c r="N73" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="O73" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="P73" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="Q73" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="R73" t="e">
         <v>#N/A</v>
       </c>
       <c r="S73" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="T73" t="e">
         <v>#N/A</v>
@@ -7335,37 +7335,37 @@
         <v>173</v>
       </c>
       <c r="H74" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I74" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="J74" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="K74" t="e">
         <v>#N/A</v>
       </c>
       <c r="L74" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="M74" t="e">
         <v>#N/A</v>
       </c>
       <c r="N74" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="O74" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="P74" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="Q74" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="R74" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="S74" t="e">
         <v>#N/A</v>
@@ -7400,34 +7400,34 @@
         <v>173</v>
       </c>
       <c r="H75" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I75" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="J75" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="K75" t="e">
         <v>#N/A</v>
       </c>
       <c r="L75" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="M75" t="e">
         <v>#N/A</v>
       </c>
       <c r="N75" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="O75" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="P75" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="Q75" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="R75" t="e">
         <v>#N/A</v>
@@ -7436,7 +7436,7 @@
         <v>#N/A</v>
       </c>
       <c r="T75" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="U75" t="s">
         <v>825</v>
@@ -7465,34 +7465,34 @@
         <v>173</v>
       </c>
       <c r="H76" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I76" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="J76" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="K76" t="e">
         <v>#N/A</v>
       </c>
       <c r="L76" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="M76" t="e">
         <v>#N/A</v>
       </c>
       <c r="N76" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="O76" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="P76" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="Q76" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="R76" t="s">
         <v>703</v>
@@ -7530,43 +7530,43 @@
         <v>173</v>
       </c>
       <c r="H77" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I77" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="J77" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="K77" t="e">
         <v>#N/A</v>
       </c>
       <c r="L77" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="M77" t="e">
         <v>#N/A</v>
       </c>
       <c r="N77" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="O77" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="P77" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="Q77" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="R77" t="s">
         <v>704</v>
       </c>
       <c r="S77" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="T77" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="U77" t="s">
         <v>827</v>
@@ -7595,37 +7595,37 @@
         <v>173</v>
       </c>
       <c r="H78" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I78" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="J78" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="K78" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="L78" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="M78" t="e">
         <v>#N/A</v>
       </c>
       <c r="N78" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="O78" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="P78" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="Q78" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="R78" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="S78" t="s">
         <v>698</v>
@@ -7660,37 +7660,37 @@
         <v>173</v>
       </c>
       <c r="H79" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="I79" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="J79" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="K79" t="e">
         <v>#N/A</v>
       </c>
       <c r="L79" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="M79" t="e">
         <v>#N/A</v>
       </c>
       <c r="N79" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="O79" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="P79" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="Q79" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="R79" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="S79" t="e">
         <v>#N/A</v>
@@ -7725,43 +7725,43 @@
         <v>173</v>
       </c>
       <c r="H80" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="I80" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="J80" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="K80" t="e">
         <v>#N/A</v>
       </c>
       <c r="L80" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="M80" t="e">
         <v>#N/A</v>
       </c>
       <c r="N80" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="O80" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="P80" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="Q80" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="R80" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="S80" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="T80" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="U80" t="s">
         <v>830</v>
@@ -7790,40 +7790,40 @@
         <v>173</v>
       </c>
       <c r="H81" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="I81" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="J81" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="K81" t="e">
         <v>#N/A</v>
       </c>
       <c r="L81" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="M81" t="e">
         <v>#N/A</v>
       </c>
       <c r="N81" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="O81" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="P81" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="Q81" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="R81" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="S81" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="T81" t="s">
         <v>745</v>
@@ -7852,46 +7852,46 @@
         <v>172</v>
       </c>
       <c r="G82" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="H82" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I82" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="J82" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="K82" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="L82" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="M82" t="e">
         <v>#N/A</v>
       </c>
       <c r="N82" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="O82" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="P82" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="Q82" t="s">
         <v>119</v>
       </c>
       <c r="R82" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="S82" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="T82" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="U82" t="s">
         <v>832</v>
@@ -7920,34 +7920,34 @@
         <v>173</v>
       </c>
       <c r="H83" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="I83" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="J83" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="K83" t="e">
         <v>#N/A</v>
       </c>
       <c r="L83" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="M83" t="e">
         <v>#N/A</v>
       </c>
       <c r="N83" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="O83" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="P83" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="Q83" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="R83" t="s">
         <v>705</v>
@@ -7985,43 +7985,43 @@
         <v>173</v>
       </c>
       <c r="H84" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="I84" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="J84" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="K84" t="e">
         <v>#N/A</v>
       </c>
       <c r="L84" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="M84" t="e">
         <v>#N/A</v>
       </c>
       <c r="N84" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="O84" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="P84" t="s">
         <v>107</v>
       </c>
       <c r="Q84" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="R84" t="s">
         <v>706</v>
       </c>
       <c r="S84" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="T84" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="U84" t="s">
         <v>834</v>

</xml_diff>